<commit_message>
Organization folder last experiment
</commit_message>
<xml_diff>
--- a/Data/1. Diving log/Diving_log_BenthFun.xlsx
+++ b/Data/1. Diving log/Diving_log_BenthFun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/1. Diving log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B00104-36C5-D144-A6B8-3A5C42B20ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF207498-7725-0347-9148-40EE20F0EAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" activeTab="1" xr2:uid="{AC65A032-FAEB-0942-B0EC-C9C433D5231F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="301">
   <si>
     <t>Diving_Date</t>
   </si>
@@ -933,6 +933,9 @@
   </si>
   <si>
     <t>Tn2_t1_AMB_blank_02</t>
+  </si>
+  <si>
+    <t>A5</t>
   </si>
 </sst>
 </file>
@@ -4111,8 +4114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8096E2FE-6459-2147-9706-235887F73F2A}">
   <dimension ref="A1:J358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="F321" sqref="F321"/>
+    <sheetView tabSelected="1" topLeftCell="A287" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13785,7 +13788,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>45185</v>
       </c>
@@ -13802,7 +13805,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
         <v>45185</v>
       </c>
@@ -13817,7 +13820,7 @@
       </c>
       <c r="H338" s="9"/>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A339" s="1">
         <v>45185</v>
       </c>
@@ -13831,7 +13834,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A340" s="1">
         <v>45185</v>
       </c>
@@ -13845,7 +13848,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
         <v>45185</v>
       </c>
@@ -13859,7 +13862,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
         <v>45185</v>
       </c>
@@ -13871,7 +13874,7 @@
       </c>
       <c r="H342" s="9"/>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A343" s="1">
         <v>45184</v>
       </c>
@@ -13881,14 +13884,29 @@
       <c r="C343" t="s">
         <v>17</v>
       </c>
+      <c r="D343" s="7">
+        <v>0.45902777777777781</v>
+      </c>
+      <c r="E343" s="7">
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="F343" s="7">
+        <v>0.50555555555555554</v>
+      </c>
       <c r="G343">
         <v>1</v>
       </c>
       <c r="H343" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I343" s="3">
+        <v>26.372</v>
+      </c>
+      <c r="J343" s="3">
+        <v>-85.6</v>
+      </c>
+    </row>
+    <row r="344" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A344" s="1">
         <v>45184</v>
       </c>
@@ -13898,14 +13916,29 @@
       <c r="C344" t="s">
         <v>18</v>
       </c>
+      <c r="D344" s="7">
+        <v>0.45624999999999999</v>
+      </c>
+      <c r="E344" s="7">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="F344" s="7">
+        <v>0.5083333333333333</v>
+      </c>
       <c r="G344">
         <v>2</v>
       </c>
       <c r="H344" s="9" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I344" s="3">
+        <v>26.443000000000001</v>
+      </c>
+      <c r="J344" s="3">
+        <v>-89.7</v>
+      </c>
+    </row>
+    <row r="345" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A345" s="1">
         <v>45184</v>
       </c>
@@ -13915,14 +13948,29 @@
       <c r="C345" t="s">
         <v>19</v>
       </c>
+      <c r="D345" s="7">
+        <v>0.45694444444444443</v>
+      </c>
+      <c r="E345" s="7">
+        <v>0.51180555555555551</v>
+      </c>
+      <c r="F345" s="7">
+        <v>0.51180555555555551</v>
+      </c>
       <c r="G345">
         <v>3</v>
       </c>
       <c r="H345" s="9" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I345" s="3">
+        <v>26.728999999999999</v>
+      </c>
+      <c r="J345" s="3">
+        <v>-80</v>
+      </c>
+    </row>
+    <row r="346" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A346" s="1">
         <v>45184</v>
       </c>
@@ -13932,64 +13980,139 @@
       <c r="C346" t="s">
         <v>20</v>
       </c>
+      <c r="D346" s="7">
+        <v>0.45763888888888887</v>
+      </c>
+      <c r="E346" s="7">
+        <v>0.51527777777777783</v>
+      </c>
+      <c r="F346" s="7">
+        <v>0.51527777777777783</v>
+      </c>
       <c r="G346">
         <v>4</v>
       </c>
-    </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I346" s="3">
+        <v>26.658000000000001</v>
+      </c>
+      <c r="J346" s="3">
+        <v>-69.400000000000006</v>
+      </c>
+    </row>
+    <row r="347" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A347" s="1">
         <v>45184</v>
       </c>
       <c r="C347" t="s">
         <v>25</v>
       </c>
+      <c r="D347" s="7">
+        <v>0.4680555555555555</v>
+      </c>
+      <c r="E347" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F347" s="7">
+        <v>0.5</v>
+      </c>
       <c r="G347">
         <v>5</v>
       </c>
       <c r="H347" s="9" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I347" s="3">
+        <v>25.715</v>
+      </c>
+      <c r="J347" s="3">
+        <v>-63.5</v>
+      </c>
+    </row>
+    <row r="348" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A348" s="1">
         <v>45184</v>
       </c>
       <c r="C348" t="s">
         <v>26</v>
       </c>
+      <c r="D348" s="7">
+        <v>0.46875</v>
+      </c>
+      <c r="E348" s="7">
+        <v>0.50069444444444444</v>
+      </c>
+      <c r="F348" s="7">
+        <v>0.50069444444444444</v>
+      </c>
       <c r="G348">
         <v>6</v>
       </c>
       <c r="H348" s="9" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I348" s="3">
+        <v>25.709</v>
+      </c>
+      <c r="J348" s="3">
+        <v>-65.400000000000006</v>
+      </c>
+    </row>
+    <row r="349" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A349" s="1">
         <v>45184</v>
       </c>
       <c r="C349" t="s">
         <v>27</v>
       </c>
+      <c r="D349" s="7">
+        <v>0.4694444444444445</v>
+      </c>
+      <c r="E349" s="7">
+        <v>0.50138888888888888</v>
+      </c>
+      <c r="F349" s="7">
+        <v>0.50138888888888888</v>
+      </c>
       <c r="G349">
         <v>7</v>
       </c>
       <c r="H349" s="9" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+      <c r="I349" s="3">
+        <v>25.853999999999999</v>
+      </c>
+      <c r="J349" s="3">
+        <v>-66.3</v>
+      </c>
+    </row>
+    <row r="350" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A350" s="1">
         <v>45184</v>
       </c>
       <c r="C350" t="s">
         <v>28</v>
       </c>
+      <c r="D350" s="7">
+        <v>0.45763888888888887</v>
+      </c>
+      <c r="E350" s="7">
+        <v>0.51527777777777783</v>
+      </c>
+      <c r="F350" s="7">
+        <v>0.51527777777777783</v>
+      </c>
       <c r="G350">
         <v>8</v>
       </c>
-    </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I350" s="3">
+        <v>26.658000000000001</v>
+      </c>
+      <c r="J350" s="3">
+        <v>-69.400000000000006</v>
+      </c>
+    </row>
+    <row r="351" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>45184</v>
       </c>
@@ -13999,14 +14122,29 @@
       <c r="C351" t="s">
         <v>21</v>
       </c>
+      <c r="D351" s="7">
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="E351" s="7">
+        <v>0.57847222222222217</v>
+      </c>
+      <c r="F351" s="7">
+        <v>0.57847222222222217</v>
+      </c>
       <c r="G351">
         <v>5</v>
       </c>
       <c r="H351" s="9" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I351" s="3">
+        <v>27.309000000000001</v>
+      </c>
+      <c r="J351" s="3">
+        <v>-81.400000000000006</v>
+      </c>
+    </row>
+    <row r="352" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
         <v>45184</v>
       </c>
@@ -14016,14 +14154,29 @@
       <c r="C352" t="s">
         <v>22</v>
       </c>
+      <c r="D352" s="7">
+        <v>0.53402777777777777</v>
+      </c>
+      <c r="E352" s="7">
+        <v>0.58263888888888882</v>
+      </c>
+      <c r="F352" s="7">
+        <v>0.58263888888888882</v>
+      </c>
       <c r="G352">
         <v>6</v>
       </c>
       <c r="H352" s="9" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I352" s="3">
+        <v>27.164999999999999</v>
+      </c>
+      <c r="J352" s="3">
+        <v>-75.8</v>
+      </c>
+    </row>
+    <row r="353" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>45184</v>
       </c>
@@ -14033,14 +14186,29 @@
       <c r="C353" t="s">
         <v>23</v>
       </c>
+      <c r="D353" s="7">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="E353" s="7">
+        <v>0.58402777777777781</v>
+      </c>
+      <c r="F353" s="7">
+        <v>0.58402777777777781</v>
+      </c>
       <c r="G353">
         <v>7</v>
       </c>
       <c r="H353" s="9" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+      <c r="I353" s="3">
+        <v>27.452999999999999</v>
+      </c>
+      <c r="J353" s="3">
+        <v>-78.7</v>
+      </c>
+    </row>
+    <row r="354" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
         <v>45184</v>
       </c>
@@ -14050,61 +14218,136 @@
       <c r="C354" t="s">
         <v>24</v>
       </c>
+      <c r="D354" s="7">
+        <v>0.53541666666666665</v>
+      </c>
+      <c r="E354" s="7">
+        <v>0.5854166666666667</v>
+      </c>
+      <c r="F354" s="7">
+        <v>0.5854166666666667</v>
+      </c>
       <c r="G354">
         <v>8</v>
       </c>
-    </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I354" s="3">
+        <v>26.984999999999999</v>
+      </c>
+      <c r="J354" s="3">
+        <v>-67.099999999999994</v>
+      </c>
+    </row>
+    <row r="355" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
         <v>45184</v>
       </c>
       <c r="C355" t="s">
         <v>29</v>
       </c>
+      <c r="D355" s="7">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E355" s="7">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="F355" s="7">
+        <v>0.57291666666666663</v>
+      </c>
       <c r="G355">
         <v>1</v>
       </c>
       <c r="H355" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I355" s="3">
+        <v>26.52</v>
+      </c>
+      <c r="J355" s="3">
+        <v>-62.6</v>
+      </c>
+    </row>
+    <row r="356" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A356" s="1">
         <v>45184</v>
       </c>
       <c r="C356" t="s">
         <v>30</v>
       </c>
+      <c r="D356" s="7">
+        <v>0.54236111111111118</v>
+      </c>
+      <c r="E356" s="7">
+        <v>0.57430555555555551</v>
+      </c>
+      <c r="F356" s="7">
+        <v>0.57430555555555551</v>
+      </c>
       <c r="G356">
         <v>2</v>
       </c>
       <c r="H356" s="9" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I356" s="3">
+        <v>26.512</v>
+      </c>
+      <c r="J356" s="3">
+        <v>-63.5</v>
+      </c>
+    </row>
+    <row r="357" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A357" s="1">
         <v>45184</v>
       </c>
       <c r="C357" t="s">
         <v>31</v>
       </c>
+      <c r="D357" s="7">
+        <v>0.54305555555555551</v>
+      </c>
+      <c r="E357" s="7">
+        <v>0.5756944444444444</v>
+      </c>
+      <c r="F357" s="7">
+        <v>0.5756944444444444</v>
+      </c>
       <c r="G357">
         <v>3</v>
       </c>
       <c r="H357" s="9" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I357" s="3">
+        <v>26.655999999999999</v>
+      </c>
+      <c r="J357" s="3">
+        <v>-61.9</v>
+      </c>
+    </row>
+    <row r="358" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A358" s="1">
         <v>45184</v>
       </c>
       <c r="C358" t="s">
         <v>32</v>
       </c>
+      <c r="D358" s="7">
+        <v>0.53541666666666665</v>
+      </c>
+      <c r="E358" s="7">
+        <v>0.5854166666666667</v>
+      </c>
+      <c r="F358" s="7">
+        <v>0.5854166666666667</v>
+      </c>
       <c r="G358">
         <v>4</v>
+      </c>
+      <c r="I358" s="3">
+        <v>26.984999999999999</v>
+      </c>
+      <c r="J358" s="3">
+        <v>-67.099999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LOW TN2 + O2 PROFILES T3 + TN2 + LIGHT PROFILE T3 + TN2 (MISSING ELOW)
</commit_message>
<xml_diff>
--- a/Data/1. Diving log/Diving_log_BenthFun.xlsx
+++ b/Data/1. Diving log/Diving_log_BenthFun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/1. Diving log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF207498-7725-0347-9148-40EE20F0EAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CC2CA9-8A97-E94F-BFEF-E22FB7B58C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" activeTab="1" xr2:uid="{AC65A032-FAEB-0942-B0EC-C9C433D5231F}"/>
   </bookViews>
@@ -4114,8 +4114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8096E2FE-6459-2147-9706-235887F73F2A}">
   <dimension ref="A1:J358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A287" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
+      <selection activeCell="L337" sqref="L337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13396,7 +13396,7 @@
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="B311" t="s">
         <v>276</v>
@@ -13413,7 +13413,7 @@
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="B312" t="s">
         <v>277</v>
@@ -13430,7 +13430,7 @@
     </row>
     <row r="313" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="B313" t="s">
         <v>278</v>
@@ -13447,7 +13447,7 @@
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="B314" t="s">
         <v>279</v>
@@ -13462,7 +13462,7 @@
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="C315" t="s">
         <v>25</v>
@@ -13476,7 +13476,7 @@
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="C316" t="s">
         <v>26</v>
@@ -13490,7 +13490,7 @@
     </row>
     <row r="317" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="C317" t="s">
         <v>27</v>
@@ -13504,7 +13504,7 @@
     </row>
     <row r="318" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="C318" t="s">
         <v>28</v>
@@ -13516,7 +13516,7 @@
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="B319" s="2" t="s">
         <v>280</v>
@@ -13533,7 +13533,7 @@
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="B320" s="2" t="s">
         <v>281</v>
@@ -13548,9 +13548,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="B321" s="2" t="s">
         <v>282</v>
@@ -13565,9 +13565,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="B322" t="s">
         <v>283</v>
@@ -13580,9 +13580,9 @@
       </c>
       <c r="H322" s="9"/>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="C323" t="s">
         <v>29</v>
@@ -13594,9 +13594,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="C324" t="s">
         <v>30</v>
@@ -13608,9 +13608,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="C325" t="s">
         <v>31</v>
@@ -13622,9 +13622,9 @@
         <v>185</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="C326" t="s">
         <v>32</v>
@@ -13634,9 +13634,9 @@
       </c>
       <c r="H326" s="9"/>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="B327" t="s">
         <v>284</v>
@@ -13644,16 +13644,31 @@
       <c r="C327" t="s">
         <v>17</v>
       </c>
+      <c r="D327" s="7">
+        <v>0.45624999999999999</v>
+      </c>
+      <c r="E327" s="7">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="F327" s="7">
+        <v>0.50277777777777777</v>
+      </c>
       <c r="G327">
         <v>1</v>
       </c>
       <c r="H327" s="9" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I327" s="3">
+        <v>26.378</v>
+      </c>
+      <c r="J327" s="3">
+        <v>-71.2</v>
+      </c>
+    </row>
+    <row r="328" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="B328" t="s">
         <v>285</v>
@@ -13661,16 +13676,31 @@
       <c r="C328" t="s">
         <v>18</v>
       </c>
+      <c r="D328" s="7">
+        <v>0.45694444444444443</v>
+      </c>
+      <c r="E328" s="7">
+        <v>0.50624999999999998</v>
+      </c>
+      <c r="F328" s="7">
+        <v>0.50624999999999998</v>
+      </c>
       <c r="G328">
         <v>2</v>
       </c>
       <c r="H328" s="9" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I328" s="3">
+        <v>26.513000000000002</v>
+      </c>
+      <c r="J328" s="3">
+        <v>-70.2</v>
+      </c>
+    </row>
+    <row r="329" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="B329" t="s">
         <v>286</v>
@@ -13678,16 +13708,31 @@
       <c r="C329" t="s">
         <v>19</v>
       </c>
+      <c r="D329" s="7">
+        <v>0.45763888888888887</v>
+      </c>
+      <c r="E329" s="7">
+        <v>0.50972222222222219</v>
+      </c>
+      <c r="F329" s="7">
+        <v>0.50972222222222219</v>
+      </c>
       <c r="G329">
         <v>3</v>
       </c>
       <c r="H329" s="9" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I329" s="3">
+        <v>26.77</v>
+      </c>
+      <c r="J329" s="3">
+        <v>-71.8</v>
+      </c>
+    </row>
+    <row r="330" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="B330" t="s">
         <v>287</v>
@@ -13695,68 +13740,143 @@
       <c r="C330" t="s">
         <v>20</v>
       </c>
+      <c r="D330" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E330" s="7">
+        <v>0.5131944444444444</v>
+      </c>
+      <c r="F330" s="7">
+        <v>0.5131944444444444</v>
+      </c>
       <c r="G330">
         <v>4</v>
       </c>
       <c r="H330" s="9"/>
-    </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I330" s="3">
+        <v>26.411999999999999</v>
+      </c>
+      <c r="J330" s="3">
+        <v>-55.5</v>
+      </c>
+    </row>
+    <row r="331" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="C331" t="s">
         <v>25</v>
       </c>
+      <c r="D331" s="7">
+        <v>0.46597222222222223</v>
+      </c>
+      <c r="E331" s="7">
+        <v>0.49791666666666662</v>
+      </c>
+      <c r="F331" s="7">
+        <v>0.49791666666666662</v>
+      </c>
       <c r="G331">
         <v>5</v>
       </c>
       <c r="H331" s="9" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I331" s="3">
+        <v>25.733000000000001</v>
+      </c>
+      <c r="J331" s="3">
+        <v>-59.3</v>
+      </c>
+    </row>
+    <row r="332" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="C332" t="s">
         <v>26</v>
       </c>
+      <c r="D332" s="7">
+        <v>0.46736111111111112</v>
+      </c>
+      <c r="E332" s="7">
+        <v>0.4993055555555555</v>
+      </c>
+      <c r="F332" s="7">
+        <v>0.4993055555555555</v>
+      </c>
       <c r="G332">
         <v>6</v>
       </c>
       <c r="H332" s="9" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I332" s="3">
+        <v>25.838000000000001</v>
+      </c>
+      <c r="J332" s="3">
+        <v>-56.5</v>
+      </c>
+    </row>
+    <row r="333" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="C333" t="s">
         <v>27</v>
       </c>
+      <c r="D333" s="7">
+        <v>0.4680555555555555</v>
+      </c>
+      <c r="E333" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F333" s="7">
+        <v>0.5</v>
+      </c>
       <c r="G333">
         <v>7</v>
       </c>
       <c r="H333" s="9" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I333" s="3">
+        <v>25.841999999999999</v>
+      </c>
+      <c r="J333" s="3">
+        <v>-58.9</v>
+      </c>
+    </row>
+    <row r="334" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="C334" t="s">
         <v>28</v>
       </c>
+      <c r="D334" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E334" s="7">
+        <v>0.5131944444444444</v>
+      </c>
+      <c r="F334" s="7">
+        <v>0.5131944444444444</v>
+      </c>
       <c r="G334">
         <v>8</v>
       </c>
       <c r="H334" s="9"/>
-    </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I334" s="3">
+        <v>26.411999999999999</v>
+      </c>
+      <c r="J334" s="3">
+        <v>-55.5</v>
+      </c>
+    </row>
+    <row r="335" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="B335" s="2" t="s">
         <v>288</v>
@@ -13764,16 +13884,31 @@
       <c r="C335" t="s">
         <v>21</v>
       </c>
+      <c r="D335" s="7">
+        <v>0.52708333333333335</v>
+      </c>
+      <c r="E335" s="7">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="F335" s="7">
+        <v>0.57291666666666663</v>
+      </c>
       <c r="G335">
         <v>5</v>
       </c>
       <c r="H335" s="9" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I335" s="3">
+        <v>26.817</v>
+      </c>
+      <c r="J335" s="3">
+        <v>-75.900000000000006</v>
+      </c>
+    </row>
+    <row r="336" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="B336" s="2" t="s">
         <v>289</v>
@@ -13781,16 +13916,31 @@
       <c r="C336" t="s">
         <v>22</v>
       </c>
+      <c r="D336" s="7">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="E336" s="7">
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="F336" s="7">
+        <v>0.57500000000000007</v>
+      </c>
       <c r="G336">
         <v>6</v>
       </c>
       <c r="H336" s="9" t="s">
         <v>209</v>
       </c>
+      <c r="I336" s="3">
+        <v>26.91</v>
+      </c>
+      <c r="J336" s="3">
+        <v>-73.2</v>
+      </c>
     </row>
     <row r="337" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="B337" s="2" t="s">
         <v>290</v>
@@ -13798,16 +13948,31 @@
       <c r="C337" t="s">
         <v>23</v>
       </c>
+      <c r="D337" s="7">
+        <v>0.52847222222222223</v>
+      </c>
+      <c r="E337" s="7">
+        <v>0.57847222222222217</v>
+      </c>
+      <c r="F337" s="7">
+        <v>0.57847222222222217</v>
+      </c>
       <c r="G337">
         <v>7</v>
       </c>
       <c r="H337" s="9" t="s">
         <v>210</v>
       </c>
+      <c r="I337" s="3">
+        <v>27.146000000000001</v>
+      </c>
+      <c r="J337" s="3">
+        <v>-77.8</v>
+      </c>
     </row>
     <row r="338" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="B338" t="s">
         <v>291</v>
@@ -13815,64 +13980,139 @@
       <c r="C338" t="s">
         <v>24</v>
       </c>
+      <c r="D338" s="7">
+        <v>0.52916666666666667</v>
+      </c>
+      <c r="E338" s="7">
+        <v>0.58194444444444449</v>
+      </c>
+      <c r="F338" s="7">
+        <v>0.58194444444444449</v>
+      </c>
       <c r="G338">
         <v>8</v>
       </c>
       <c r="H338" s="9"/>
+      <c r="I338" s="3">
+        <v>27.056000000000001</v>
+      </c>
+      <c r="J338" s="3">
+        <v>-62</v>
+      </c>
     </row>
     <row r="339" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A339" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="C339" t="s">
         <v>29</v>
       </c>
+      <c r="D339" s="7">
+        <v>0.53611111111111109</v>
+      </c>
+      <c r="E339" s="7">
+        <v>0.56805555555555554</v>
+      </c>
+      <c r="F339" s="7">
+        <v>0.56805555555555554</v>
+      </c>
       <c r="G339">
         <v>1</v>
       </c>
       <c r="H339" s="9" t="s">
         <v>205</v>
       </c>
+      <c r="I339" s="3">
+        <v>26.405000000000001</v>
+      </c>
+      <c r="J339" s="3">
+        <v>-60.9</v>
+      </c>
     </row>
     <row r="340" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A340" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="C340" t="s">
         <v>30</v>
       </c>
+      <c r="D340" s="7">
+        <v>0.53680555555555554</v>
+      </c>
+      <c r="E340" s="7">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="F340" s="7">
+        <v>0.56944444444444442</v>
+      </c>
       <c r="G340">
         <v>2</v>
       </c>
       <c r="H340" s="9" t="s">
         <v>206</v>
       </c>
+      <c r="I340" s="3">
+        <v>26.393000000000001</v>
+      </c>
+      <c r="J340" s="3">
+        <v>-62.5</v>
+      </c>
     </row>
     <row r="341" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="C341" t="s">
         <v>31</v>
       </c>
+      <c r="D341" s="7">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="E341" s="7">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="F341" s="7">
+        <v>0.56944444444444442</v>
+      </c>
       <c r="G341">
         <v>3</v>
       </c>
       <c r="H341" s="9" t="s">
         <v>207</v>
       </c>
+      <c r="I341" s="3">
+        <v>26.509</v>
+      </c>
+      <c r="J341" s="3">
+        <v>-64.400000000000006</v>
+      </c>
     </row>
     <row r="342" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="C342" t="s">
         <v>32</v>
       </c>
+      <c r="D342" s="7">
+        <v>0.52916666666666667</v>
+      </c>
+      <c r="E342" s="7">
+        <v>0.58194444444444449</v>
+      </c>
+      <c r="F342" s="7">
+        <v>0.58194444444444449</v>
+      </c>
       <c r="G342">
         <v>4</v>
       </c>
       <c r="H342" s="9"/>
+      <c r="I342" s="3">
+        <v>27.056000000000001</v>
+      </c>
+      <c r="J342" s="3">
+        <v>-62</v>
+      </c>
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A343" s="1">

</xml_diff>